<commit_message>
map of L list
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellis\Documents\projects\Numerical-Alg-Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6FF2DB-0127-4449-81C2-1F930B835472}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFF4D5E-29FC-4AEC-A5D3-4924B33B44B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29295" yWindow="450" windowWidth="13395" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -36,10 +36,19 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Could be done but need to confirm answer</t>
-  </si>
-  <si>
-    <t>Done</t>
+    <t>1 Central Difference</t>
+  </si>
+  <si>
+    <t>Report will be long</t>
+  </si>
+  <si>
+    <t>2 Coordinates</t>
+  </si>
+  <si>
+    <t>3 Central vs richardson</t>
+  </si>
+  <si>
+    <t>4 Romberg</t>
   </si>
 </sst>
 </file>
@@ -378,12 +387,12 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" customWidth="1"/>
   </cols>
@@ -400,42 +409,42 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -448,7 +457,9 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
       <c r="C7" s="2"/>
     </row>
   </sheetData>

</xml_diff>